<commit_message>
change requirement file and test data
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alireza\Documents\uni\Emailresan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1FD2D4-C34E-4FF0-8FA4-AF32B810C7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE76E10-983B-4582-BC31-79A2410BD620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,13 +39,13 @@
     <t>alireza</t>
   </si>
   <si>
-    <t>ali@gmail.com</t>
-  </si>
-  <si>
-    <t>sara@gmail.com</t>
-  </si>
-  <si>
     <t>sara</t>
+  </si>
+  <si>
+    <t>alireza.13rafe@gmail.com</t>
+  </si>
+  <si>
+    <t>alireza.00gaming@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -398,21 +398,22 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{095F51B2-CD28-44C0-A595-D6AD6167CB84}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{7BCD0DFA-3B5C-4265-B5D0-219674BC1201}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>